<commit_message>
add buttons functionality, download result, and other features
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -1,37 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A599D384-568E-674E-B8DE-05E44CFC37F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="18860" windowHeight="16140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="18860" windowHeight="16140" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="enabling_environment" sheetId="3" r:id="rId1"/>
-    <sheet name="market_creation" sheetId="1" r:id="rId2"/>
-    <sheet name="organisational_change" sheetId="2" r:id="rId3"/>
-    <sheet name="all" sheetId="4" r:id="rId4"/>
+    <sheet sheetId="3" name="enabling_environment" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="market_creation" state="visible" r:id="rId5"/>
+    <sheet sheetId="2" name="organisational_change" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="all" state="visible" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
@@ -39,6 +25,12 @@
     <t>email</t>
   </si>
   <si>
+    <t>org_name</t>
+  </si>
+  <si>
+    <t>org_type</t>
+  </si>
+  <si>
     <t>q1</t>
   </si>
   <si>
@@ -81,6 +73,18 @@
     <t>ee_result</t>
   </si>
   <si>
+    <t>Angleina Rianti</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>q4</t>
   </si>
   <si>
@@ -123,9 +127,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Partially</t>
   </si>
   <si>
@@ -180,33 +181,39 @@
     <t>oc_result</t>
   </si>
   <si>
+    <t>Angelina Rianti</t>
+  </si>
+  <si>
+    <t>angelinarianti23@gmail.com</t>
+  </si>
+  <si>
+    <t>Swinburne</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
     <t>business_category</t>
-  </si>
-  <si>
-    <t>org_name</t>
-  </si>
-  <si>
-    <t>org_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -547,16 +554,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="16" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,52 +571,69 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" ht="16" customHeight="1" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -618,16 +642,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="16" customHeight="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -635,69 +659,108 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
+      <c r="R1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>28</v>
+      <c r="S1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -706,16 +769,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="16" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -723,58 +786,130 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>48</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -783,19 +918,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
   <cols>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="16" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -803,19 +938,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>